<commit_message>
finished clock algorithm, and completed gathering data for it. next up is the aging algorithm.
</commit_message>
<xml_diff>
--- a/project03/SimulationOutputs.xlsx
+++ b/project03/SimulationOutputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="3600" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="8900" yWindow="3100" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="10">
   <si>
     <t>ALGORITHM</t>
   </si>
@@ -47,12 +47,15 @@
   <si>
     <t>gcc.trace</t>
   </si>
+  <si>
+    <t>CLOCK</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -84,8 +87,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,8 +114,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -128,15 +144,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -144,13 +189,34 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -480,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G16"/>
+  <dimension ref="B3:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -677,54 +743,164 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2">
+        <v>8</v>
+      </c>
       <c r="D12" s="2">
         <v>999999</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="E12" s="2">
+        <v>265691</v>
+      </c>
+      <c r="F12" s="2">
+        <v>55664</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2">
+        <v>16</v>
+      </c>
       <c r="D13" s="2">
         <v>999999</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="E13" s="2">
+        <v>136154</v>
+      </c>
+      <c r="F13" s="2">
+        <v>52104</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2">
+        <v>32</v>
+      </c>
       <c r="D14" s="2">
         <v>999999</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="E14" s="2">
+        <v>73924</v>
+      </c>
+      <c r="F14" s="2">
+        <v>45872</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2">
+        <v>64</v>
+      </c>
       <c r="D15" s="2">
         <v>999999</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="E15" s="2">
+        <v>56974</v>
+      </c>
+      <c r="F15" s="3">
+        <v>43965</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2">
+        <v>8</v>
+      </c>
       <c r="D16" s="2">
         <v>999999</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="E16" s="2">
+        <v>178111</v>
+      </c>
+      <c r="F16" s="4">
+        <v>38992</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E17" s="2">
+        <v>122579</v>
+      </c>
+      <c r="F17" s="4">
+        <v>26633</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2">
+        <v>32</v>
+      </c>
+      <c r="D18" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E18" s="2">
+        <v>88457</v>
+      </c>
+      <c r="F18" s="4">
+        <v>20193</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2">
+        <v>64</v>
+      </c>
+      <c r="D19" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E19" s="2">
+        <v>61832</v>
+      </c>
+      <c r="F19" s="4">
+        <v>15840</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
finished all algorithms, gathered data. next need to create graphs, do written portion of project. and clean code for submission.
</commit_message>
<xml_diff>
--- a/project03/SimulationOutputs.xlsx
+++ b/project03/SimulationOutputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8900" yWindow="3100" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="4920" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="20">
   <si>
     <t>ALGORITHM</t>
   </si>
@@ -49,13 +49,43 @@
   </si>
   <si>
     <t>CLOCK</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>AGING</t>
+  </si>
+  <si>
+    <t>1ms</t>
+  </si>
+  <si>
+    <t>REFRESH RATE</t>
+  </si>
+  <si>
+    <t>0.001ms</t>
+  </si>
+  <si>
+    <t>100ms</t>
+  </si>
+  <si>
+    <t>TEST FOR BEST REFRESH RATE</t>
+  </si>
+  <si>
+    <t>0.000001ms</t>
+  </si>
+  <si>
+    <t>100000ms</t>
+  </si>
+  <si>
+    <t>LRU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -67,6 +97,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -158,30 +196,70 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,14 +267,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -207,6 +286,26 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -217,6 +316,26 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -546,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G19"/>
+  <dimension ref="B3:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -560,9 +679,15 @@
     <col min="5" max="5" width="28.1640625" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" customWidth="1"/>
     <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="12" max="12" width="25" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" customWidth="1"/>
+    <col min="14" max="14" width="22" customWidth="1"/>
+    <col min="16" max="16" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:16">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,8 +706,14 @@
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:7">
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -601,8 +732,32 @@
       <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:7">
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -621,8 +776,32 @@
       <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="2:7">
+      <c r="H5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="2">
+        <v>8</v>
+      </c>
+      <c r="L5" s="2">
+        <v>999999</v>
+      </c>
+      <c r="M5" s="2">
+        <v>275255</v>
+      </c>
+      <c r="N5" s="2">
+        <v>53874</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -641,8 +820,32 @@
       <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="2:7">
+      <c r="H6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="2">
+        <v>8</v>
+      </c>
+      <c r="L6" s="2">
+        <v>999999</v>
+      </c>
+      <c r="M6" s="2">
+        <v>275255</v>
+      </c>
+      <c r="N6" s="2">
+        <v>53874</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -661,8 +864,32 @@
       <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="2:7">
+      <c r="H7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="2">
+        <v>8</v>
+      </c>
+      <c r="L7" s="2">
+        <v>999999</v>
+      </c>
+      <c r="M7" s="2">
+        <v>275356</v>
+      </c>
+      <c r="N7" s="2">
+        <v>53861</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -681,8 +908,32 @@
       <c r="G8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="2:7">
+      <c r="H8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="2">
+        <v>8</v>
+      </c>
+      <c r="L8" s="2">
+        <v>999999</v>
+      </c>
+      <c r="M8" s="2">
+        <v>295001</v>
+      </c>
+      <c r="N8" s="2">
+        <v>53832</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
@@ -701,8 +952,32 @@
       <c r="G9" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:7">
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="2">
+        <v>8</v>
+      </c>
+      <c r="L9" s="2">
+        <v>999999</v>
+      </c>
+      <c r="M9" s="2">
+        <v>626895</v>
+      </c>
+      <c r="N9" s="2">
+        <v>57379</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16">
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
@@ -721,8 +996,11 @@
       <c r="G10" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:7">
+      <c r="H10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
@@ -741,8 +1019,11 @@
       <c r="G11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="2:7">
+      <c r="H11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16">
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
@@ -761,8 +1042,11 @@
       <c r="G12" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="2:7">
+      <c r="H12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -781,8 +1065,11 @@
       <c r="G13" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="2:7">
+      <c r="H13" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16">
       <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
@@ -801,8 +1088,11 @@
       <c r="G14" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="2:7">
+      <c r="H14" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16">
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -821,8 +1111,11 @@
       <c r="G15" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="2:7">
+      <c r="H15" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
@@ -841,8 +1134,11 @@
       <c r="G16" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="2:7">
+      <c r="H16" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
       <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
@@ -861,8 +1157,11 @@
       <c r="G17" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="2:7">
+      <c r="H17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
@@ -881,8 +1180,11 @@
       <c r="G18" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="2:7">
+      <c r="H18" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
       <c r="B19" s="2" t="s">
         <v>9</v>
       </c>
@@ -900,6 +1202,373 @@
       </c>
       <c r="G19" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E20" s="2">
+        <v>275255</v>
+      </c>
+      <c r="F20" s="2">
+        <v>53874</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2">
+        <v>16</v>
+      </c>
+      <c r="D21" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E21" s="2">
+        <v>244515</v>
+      </c>
+      <c r="F21" s="2">
+        <v>52162</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2">
+        <v>32</v>
+      </c>
+      <c r="D22" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E22" s="2">
+        <v>208493</v>
+      </c>
+      <c r="F22" s="2">
+        <v>50524</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="2">
+        <v>64</v>
+      </c>
+      <c r="D23" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E23" s="2">
+        <v>197510</v>
+      </c>
+      <c r="F23" s="3">
+        <v>49407</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="2">
+        <v>8</v>
+      </c>
+      <c r="D24" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E24" s="2">
+        <v>193004</v>
+      </c>
+      <c r="F24" s="4">
+        <v>33277</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="2">
+        <v>16</v>
+      </c>
+      <c r="D25" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E25" s="2">
+        <v>183624</v>
+      </c>
+      <c r="F25" s="4">
+        <v>29193</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="2">
+        <v>32</v>
+      </c>
+      <c r="D26" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E26" s="2">
+        <v>172992</v>
+      </c>
+      <c r="F26" s="4">
+        <v>25669</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="2">
+        <v>64</v>
+      </c>
+      <c r="D27" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E27" s="2">
+        <v>162486</v>
+      </c>
+      <c r="F27" s="4">
+        <v>19795</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="2">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E28" s="2">
+        <v>274323</v>
+      </c>
+      <c r="F28" s="2">
+        <v>55138</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="2">
+        <v>16</v>
+      </c>
+      <c r="D29" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E29" s="2">
+        <v>143477</v>
+      </c>
+      <c r="F29" s="2">
+        <v>47598</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="2">
+        <v>32</v>
+      </c>
+      <c r="D30" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E30" s="2">
+        <v>75235</v>
+      </c>
+      <c r="F30" s="2">
+        <v>43950</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="2">
+        <v>64</v>
+      </c>
+      <c r="D31" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E31" s="2">
+        <v>57180</v>
+      </c>
+      <c r="F31" s="2">
+        <v>43026</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="2">
+        <v>8</v>
+      </c>
+      <c r="D32" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E32" s="2">
+        <v>181950</v>
+      </c>
+      <c r="F32" s="2">
+        <v>37239</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="2">
+        <v>16</v>
+      </c>
+      <c r="D33" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E33" s="2">
+        <v>124267</v>
+      </c>
+      <c r="F33" s="2">
+        <v>23639</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="2">
+        <v>32</v>
+      </c>
+      <c r="D34" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E34" s="2">
+        <v>88992</v>
+      </c>
+      <c r="F34" s="2">
+        <v>17107</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="2">
+        <v>64</v>
+      </c>
+      <c r="D35" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
program debugged. next need to package for submission, and write the accompanying report
</commit_message>
<xml_diff>
--- a/project03/SimulationOutputs.xlsx
+++ b/project03/SimulationOutputs.xlsx
@@ -1567,7 +1567,7 @@
                   <c:v>83827.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58467.0</c:v>
+                  <c:v>58468.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1789,7 +1789,7 @@
                   <c:v>14159.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9917.0</c:v>
+                  <c:v>9916.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2734,8 +2734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3083,10 +3083,10 @@
         <v>1000000</v>
       </c>
       <c r="E11" s="3">
-        <v>58467</v>
+        <v>58468</v>
       </c>
       <c r="F11" s="3">
-        <v>9917</v>
+        <v>9916</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
fixed error with converting to float for aging algorithm
</commit_message>
<xml_diff>
--- a/project03/SimulationOutputs.xlsx
+++ b/project03/SimulationOutputs.xlsx
@@ -274,8 +274,70 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -373,7 +435,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="131">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -408,6 +470,37 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -442,6 +535,37 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2054,15 +2178,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$M$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TOTAL PAGE FAULTS </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Swim.trace</c:v>
           </c:tx>
           <c:cat>
             <c:strRef>
@@ -2734,8 +2850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="AQ12" sqref="AQ12:AW17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2752,6 +2868,7 @@
     <col min="13" max="13" width="17.83203125" customWidth="1"/>
     <col min="14" max="14" width="22" customWidth="1"/>
     <col min="16" max="16" width="19.83203125" customWidth="1"/>
+    <col min="37" max="43" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16">

</xml_diff>

<commit_message>
prepare for final submission
</commit_message>
<xml_diff>
--- a/project03/SimulationOutputs.xlsx
+++ b/project03/SimulationOutputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6160" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="1380" yWindow="1780" windowWidth="22420" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="50">
   <si>
     <t>ALGORITHM</t>
   </si>
@@ -57,24 +57,12 @@
     <t>AGING</t>
   </si>
   <si>
-    <t>1ms</t>
-  </si>
-  <si>
     <t>REFRESH RATE</t>
   </si>
   <si>
     <t>0.001ms</t>
   </si>
   <si>
-    <t>100ms</t>
-  </si>
-  <si>
-    <t>0.000001ms</t>
-  </si>
-  <si>
-    <t>100000ms</t>
-  </si>
-  <si>
     <t>LRU</t>
   </si>
   <si>
@@ -145,6 +133,42 @@
   </si>
   <si>
     <t>AGING ALGORITHM - DISK WRITES/REFRESH RATE</t>
+  </si>
+  <si>
+    <t>0.00001ms</t>
+  </si>
+  <si>
+    <t>3 zeros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 zeros </t>
+  </si>
+  <si>
+    <t>1 zero</t>
+  </si>
+  <si>
+    <t>4 zeros</t>
+  </si>
+  <si>
+    <t>16 frames</t>
+  </si>
+  <si>
+    <t>32 frames</t>
+  </si>
+  <si>
+    <t>64 frames</t>
+  </si>
+  <si>
+    <t>8 frames</t>
+  </si>
+  <si>
+    <t>0.0001ms</t>
+  </si>
+  <si>
+    <t>0.01ms</t>
+  </si>
+  <si>
+    <t>0.1ms</t>
   </si>
 </sst>
 </file>
@@ -199,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +258,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -274,7 +304,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="131">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -406,8 +436,60 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -434,8 +516,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="131">
+  <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -501,6 +587,32 @@
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -566,6 +678,32 @@
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -605,19 +743,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.000001ms</c:v>
+                  <c:v>0.00001ms</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.0001ms</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.001ms</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1ms</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>100ms</c:v>
+                  <c:v>0.01ms</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000ms</c:v>
+                  <c:v>0.1ms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -629,19 +767,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>275255.0</c:v>
+                  <c:v>275329.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275255.0</c:v>
+                  <c:v>274915.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>275356.0</c:v>
+                  <c:v>268775.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>295001.0</c:v>
+                  <c:v>257952.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>626895.0</c:v>
+                  <c:v>278471.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -660,19 +798,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.000001ms</c:v>
+                  <c:v>0.00001ms</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.0001ms</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.001ms</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1ms</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>100ms</c:v>
+                  <c:v>0.01ms</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000ms</c:v>
+                  <c:v>0.1ms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -684,19 +822,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>53874.0</c:v>
+                  <c:v>53883.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53874.0</c:v>
+                  <c:v>53882.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53861.0</c:v>
+                  <c:v>53540.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53832.0</c:v>
+                  <c:v>52664.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57379.0</c:v>
+                  <c:v>56527.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -713,20 +851,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2115909896"/>
-        <c:axId val="-2115915240"/>
+        <c:axId val="2131215368"/>
+        <c:axId val="2131218312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2115909896"/>
+        <c:axId val="2131215368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115915240"/>
+        <c:crossAx val="2131218312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -734,7 +873,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115915240"/>
+        <c:axId val="2131218312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,7 +884,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115909896"/>
+        <c:crossAx val="2131215368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -799,19 +938,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.000001ms</c:v>
+                  <c:v>0.00001ms</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.0001ms</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.001ms</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1ms</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>100ms</c:v>
+                  <c:v>0.01ms</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000ms</c:v>
+                  <c:v>0.1ms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -823,19 +962,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>275255.0</c:v>
+                  <c:v>275329.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275255.0</c:v>
+                  <c:v>274915.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>275356.0</c:v>
+                  <c:v>268775.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>295001.0</c:v>
+                  <c:v>257952.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>626895.0</c:v>
+                  <c:v>278471.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -855,19 +994,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>193004.0</c:v>
+                  <c:v>192916.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>193004.0</c:v>
+                  <c:v>192238.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>193077.0</c:v>
+                  <c:v>197848.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>229058.0</c:v>
+                  <c:v>244951.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>716028.0</c:v>
+                  <c:v>339636.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -884,20 +1023,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2111907400"/>
-        <c:axId val="-2111905672"/>
+        <c:axId val="2129810488"/>
+        <c:axId val="2129807496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2111907400"/>
+        <c:axId val="2129810488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111905672"/>
+        <c:crossAx val="2129807496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -905,7 +1045,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111905672"/>
+        <c:axId val="2129807496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -916,7 +1056,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111907400"/>
+        <c:crossAx val="2129810488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -970,19 +1110,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.000001ms</c:v>
+                  <c:v>0.00001ms</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.0001ms</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.001ms</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1ms</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>100ms</c:v>
+                  <c:v>0.01ms</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000ms</c:v>
+                  <c:v>0.1ms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -994,19 +1134,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>53874.0</c:v>
+                  <c:v>53883.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53874.0</c:v>
+                  <c:v>53882.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53861.0</c:v>
+                  <c:v>53540.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53832.0</c:v>
+                  <c:v>52664.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57379.0</c:v>
+                  <c:v>56527.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1026,19 +1166,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>33277.0</c:v>
+                  <c:v>33295.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33277.0</c:v>
+                  <c:v>33176.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33317.0</c:v>
+                  <c:v>31375.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39292.0</c:v>
+                  <c:v>31227.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>104924.0</c:v>
+                  <c:v>40763.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1055,20 +1195,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2109105672"/>
-        <c:axId val="-2114311928"/>
+        <c:axId val="2131227112"/>
+        <c:axId val="2131230056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2109105672"/>
+        <c:axId val="2131227112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114311928"/>
+        <c:crossAx val="2131230056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1076,7 +1217,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114311928"/>
+        <c:axId val="2131230056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1087,7 +1228,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109105672"/>
+        <c:crossAx val="2131227112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1272,16 +1413,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>275255.0</c:v>
+                  <c:v>257952.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>244515.0</c:v>
+                  <c:v>143989.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>208493.0</c:v>
+                  <c:v>91852.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>197510.0</c:v>
+                  <c:v>82288.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1351,11 +1492,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114918408"/>
-        <c:axId val="-2109465704"/>
+        <c:axId val="2131274024"/>
+        <c:axId val="2131277144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114918408"/>
+        <c:axId val="2131274024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1365,7 +1506,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109465704"/>
+        <c:crossAx val="2131277144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1373,7 +1514,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2109465704"/>
+        <c:axId val="2131277144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1384,7 +1525,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114918408"/>
+        <c:crossAx val="2131274024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1518,16 +1659,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>53874.0</c:v>
+                  <c:v>52664.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52162.0</c:v>
+                  <c:v>41902.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50524.0</c:v>
+                  <c:v>29993.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49407.0</c:v>
+                  <c:v>27601.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1573,11 +1714,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2108140952"/>
-        <c:axId val="-2111536232"/>
+        <c:axId val="2131308088"/>
+        <c:axId val="2131311208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2108140952"/>
+        <c:axId val="2131308088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1587,7 +1728,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111536232"/>
+        <c:crossAx val="2131311208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1595,7 +1736,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111536232"/>
+        <c:axId val="2131311208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1606,7 +1747,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108140952"/>
+        <c:crossAx val="2131308088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1740,16 +1881,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>193004.0</c:v>
+                  <c:v>244951.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>183624.0</c:v>
+                  <c:v>187385.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>172992.0</c:v>
+                  <c:v>161117.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>162486.0</c:v>
+                  <c:v>149414.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1795,11 +1936,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2112037016"/>
-        <c:axId val="-2112606232"/>
+        <c:axId val="2131343160"/>
+        <c:axId val="2131346280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2112037016"/>
+        <c:axId val="2131343160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1809,7 +1950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112606232"/>
+        <c:crossAx val="2131346280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1817,7 +1958,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112606232"/>
+        <c:axId val="2131346280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1828,7 +1969,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112037016"/>
+        <c:crossAx val="2131343160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2004,16 +2145,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>33277.0</c:v>
+                  <c:v>31227.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29193.0</c:v>
+                  <c:v>22721.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25669.0</c:v>
+                  <c:v>19519.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19795.0</c:v>
+                  <c:v>16800.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2080,11 +2221,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2110901848"/>
-        <c:axId val="-2111585512"/>
+        <c:axId val="2131379720"/>
+        <c:axId val="2131382840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2110901848"/>
+        <c:axId val="2131379720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2094,7 +2235,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111585512"/>
+        <c:crossAx val="2131382840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2102,7 +2243,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111585512"/>
+        <c:axId val="2131382840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2113,7 +2254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110901848"/>
+        <c:crossAx val="2131379720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2182,35 +2323,47 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$P$5:$P$7</c:f>
+              <c:f>Sheet1!$P$5:$P$9</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.000001ms</c:v>
+                  <c:v>0.00001ms</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.0001ms</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.001ms</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1ms</c:v>
+                <c:pt idx="3">
+                  <c:v>0.01ms</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1ms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$5:$M$7</c:f>
+              <c:f>Sheet1!$M$5:$M$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>275255.0</c:v>
+                  <c:v>275329.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275255.0</c:v>
+                  <c:v>274915.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>275356.0</c:v>
+                  <c:v>268775.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>257952.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>278471.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2227,20 +2380,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114804136"/>
-        <c:axId val="-2109614280"/>
+        <c:axId val="2131404248"/>
+        <c:axId val="2131407192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114804136"/>
+        <c:axId val="2131404248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109614280"/>
+        <c:crossAx val="2131407192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2248,7 +2402,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2109614280"/>
+        <c:axId val="2131407192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2259,7 +2413,170 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114804136"/>
+        <c:crossAx val="2131404248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>TOTAL</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> PAGE FAULTS - DETAIL</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>GCC.TRACE</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$P$52:$P$57</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.00001ms</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0001ms</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.001ms</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01ms</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$52:$M$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>192916.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>192238.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>197848.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>244951.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>339636.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2128734568"/>
+        <c:axId val="2137972792"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2128734568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2137972792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2137972792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2128734568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2518,6 +2835,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1504950</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2848,10 +3195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P89"/>
+  <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="AQ12" sqref="AQ12:AW17"/>
+    <sheetView tabSelected="1" topLeftCell="I28" workbookViewId="0">
+      <selection activeCell="M56" sqref="M52:M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2871,12 +3218,12 @@
     <col min="37" max="43" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16">
+    <row r="1" spans="2:21">
       <c r="B1" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2896,13 +3243,22 @@
         <v>6</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16">
+        <v>15</v>
+      </c>
+      <c r="S3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="T3">
+        <v>275329</v>
+      </c>
+      <c r="U3">
+        <v>53883</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -2943,10 +3299,19 @@
         <v>6</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16">
+        <v>12</v>
+      </c>
+      <c r="S4">
+        <v>1E-4</v>
+      </c>
+      <c r="T4">
+        <v>274915</v>
+      </c>
+      <c r="U4">
+        <v>53882</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2978,19 +3343,28 @@
         <v>1000000</v>
       </c>
       <c r="M5" s="3">
-        <v>275255</v>
+        <v>275329</v>
       </c>
       <c r="N5" s="3">
-        <v>53874</v>
+        <v>53883</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16">
+      <c r="P5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="S5">
+        <v>1E-3</v>
+      </c>
+      <c r="T5">
+        <v>268775</v>
+      </c>
+      <c r="U5">
+        <v>53540</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -3022,19 +3396,28 @@
         <v>1000000</v>
       </c>
       <c r="M6" s="3">
-        <v>275255</v>
+        <v>274915</v>
       </c>
       <c r="N6" s="3">
-        <v>53874</v>
+        <v>53882</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16">
+      <c r="P6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6">
+        <v>0.01</v>
+      </c>
+      <c r="T6">
+        <v>257952</v>
+      </c>
+      <c r="U6">
+        <v>52664</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -3066,19 +3449,28 @@
         <v>1000000</v>
       </c>
       <c r="M7" s="3">
-        <v>275356</v>
+        <v>268775</v>
       </c>
       <c r="N7" s="3">
-        <v>53861</v>
+        <v>53540</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16">
+      <c r="P7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="S7">
+        <v>0.1</v>
+      </c>
+      <c r="T7">
+        <v>278471</v>
+      </c>
+      <c r="U7">
+        <v>56527</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
@@ -3110,19 +3502,28 @@
         <v>1000000</v>
       </c>
       <c r="M8" s="3">
-        <v>295001</v>
+        <v>257952</v>
       </c>
       <c r="N8" s="3">
-        <v>53832</v>
+        <v>52664</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16">
+      <c r="P8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>309280</v>
+      </c>
+      <c r="U8">
+        <v>57251</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21">
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
@@ -3154,19 +3555,19 @@
         <v>1000000</v>
       </c>
       <c r="M9" s="3">
-        <v>626895</v>
+        <v>278471</v>
       </c>
       <c r="N9" s="3">
-        <v>57379</v>
+        <v>56527</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P9" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16">
+      <c r="P9" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21">
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
@@ -3188,8 +3589,11 @@
       <c r="H10" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="2:16">
+      <c r="R10">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21">
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
@@ -3211,8 +3615,17 @@
       <c r="H11" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="2:16">
+      <c r="S11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T11">
+        <v>257952</v>
+      </c>
+      <c r="U11">
+        <v>52664</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21">
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
@@ -3234,8 +3647,17 @@
       <c r="H12" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="2:16">
+      <c r="S12" t="s">
+        <v>43</v>
+      </c>
+      <c r="T12">
+        <v>143989</v>
+      </c>
+      <c r="U12">
+        <v>41902</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21">
       <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
@@ -3258,13 +3680,22 @@
         <v>10</v>
       </c>
       <c r="J13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16">
+        <v>33</v>
+      </c>
+      <c r="S13" t="s">
+        <v>44</v>
+      </c>
+      <c r="T13">
+        <v>91852</v>
+      </c>
+      <c r="U13">
+        <v>29993</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21">
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
@@ -3286,8 +3717,17 @@
       <c r="H14" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="2:16">
+      <c r="S14" t="s">
+        <v>45</v>
+      </c>
+      <c r="T14">
+        <v>82288</v>
+      </c>
+      <c r="U14">
+        <v>27601</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21">
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -3310,7 +3750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:21">
       <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
@@ -3369,7 +3809,7 @@
       <c r="E18" s="3">
         <v>88457</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="11">
         <v>20193</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -3392,7 +3832,7 @@
       <c r="E19" s="3">
         <v>61832</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="11">
         <v>15840</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -3413,16 +3853,16 @@
         <v>1000000</v>
       </c>
       <c r="E20" s="3">
-        <v>275255</v>
+        <v>257952</v>
       </c>
       <c r="F20" s="3">
-        <v>53874</v>
+        <v>52664</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="2:14">
@@ -3436,16 +3876,16 @@
         <v>1000000</v>
       </c>
       <c r="E21" s="3">
-        <v>244515</v>
+        <v>143989</v>
       </c>
       <c r="F21" s="3">
-        <v>52162</v>
+        <v>41902</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="2:14">
@@ -3459,16 +3899,16 @@
         <v>1000000</v>
       </c>
       <c r="E22" s="3">
-        <v>208493</v>
+        <v>91852</v>
       </c>
       <c r="F22" s="3">
-        <v>50524</v>
+        <v>29993</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="2:14">
@@ -3482,16 +3922,16 @@
         <v>1000000</v>
       </c>
       <c r="E23" s="3">
-        <v>197510</v>
-      </c>
-      <c r="F23" s="4">
-        <v>49407</v>
+        <v>82288</v>
+      </c>
+      <c r="F23" s="3">
+        <v>27601</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="2:14">
@@ -3505,16 +3945,16 @@
         <v>1000000</v>
       </c>
       <c r="E24" s="3">
-        <v>193004</v>
-      </c>
-      <c r="F24" s="5">
-        <v>33277</v>
+        <v>244951</v>
+      </c>
+      <c r="F24" s="3">
+        <v>31227</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="2:14">
@@ -3528,16 +3968,16 @@
         <v>1000000</v>
       </c>
       <c r="E25" s="3">
-        <v>183624</v>
-      </c>
-      <c r="F25" s="5">
-        <v>29193</v>
+        <v>187385</v>
+      </c>
+      <c r="F25" s="3">
+        <v>22721</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="2:14">
@@ -3551,16 +3991,16 @@
         <v>1000000</v>
       </c>
       <c r="E26" s="3">
-        <v>172992</v>
-      </c>
-      <c r="F26" s="5">
-        <v>25669</v>
+        <v>161117</v>
+      </c>
+      <c r="F26" s="3">
+        <v>19519</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="2:14">
@@ -3574,21 +4014,21 @@
         <v>1000000</v>
       </c>
       <c r="E27" s="3">
-        <v>162486</v>
-      </c>
-      <c r="F27" s="5">
-        <v>19795</v>
+        <v>149414</v>
+      </c>
+      <c r="F27" s="3">
+        <v>16800</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="2:14">
       <c r="B28" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C28" s="3">
         <v>8</v>
@@ -3611,7 +4051,7 @@
     </row>
     <row r="29" spans="2:14">
       <c r="B29" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C29" s="3">
         <v>16</v>
@@ -3634,7 +4074,7 @@
     </row>
     <row r="30" spans="2:14">
       <c r="B30" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C30" s="3">
         <v>32</v>
@@ -3657,7 +4097,7 @@
     </row>
     <row r="31" spans="2:14">
       <c r="B31" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C31" s="3">
         <v>64</v>
@@ -3680,7 +4120,7 @@
     </row>
     <row r="32" spans="2:14">
       <c r="B32" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C32" s="3">
         <v>8</v>
@@ -3701,15 +4141,15 @@
         <v>10</v>
       </c>
       <c r="K32" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="N32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C33" s="3">
         <v>16</v>
@@ -3732,7 +4172,7 @@
     </row>
     <row r="34" spans="2:8">
       <c r="B34" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C34" s="3">
         <v>32</v>
@@ -3755,7 +4195,7 @@
     </row>
     <row r="35" spans="2:8">
       <c r="B35" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C35" s="3">
         <v>64</v>
@@ -3778,15 +4218,15 @@
     </row>
     <row r="38" spans="2:8">
       <c r="B38" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="2:16">
       <c r="J50" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="2:16">
@@ -3809,7 +4249,7 @@
         <v>6</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="2:16">
@@ -3823,16 +4263,16 @@
         <v>1000000</v>
       </c>
       <c r="M52" s="3">
-        <v>193004</v>
+        <v>192916</v>
       </c>
       <c r="N52" s="3">
-        <v>33277</v>
+        <v>33295</v>
       </c>
       <c r="O52" s="3" t="s">
         <v>8</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="2:16">
@@ -3846,16 +4286,16 @@
         <v>1000000</v>
       </c>
       <c r="M53" s="3">
-        <v>193004</v>
+        <v>192238</v>
       </c>
       <c r="N53" s="3">
-        <v>33277</v>
+        <v>33176</v>
       </c>
       <c r="O53" s="3" t="s">
         <v>8</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="2:16">
@@ -3869,16 +4309,16 @@
         <v>1000000</v>
       </c>
       <c r="M54" s="3">
-        <v>193077</v>
+        <v>197848</v>
       </c>
       <c r="N54" s="3">
-        <v>33317</v>
+        <v>31375</v>
       </c>
       <c r="O54" s="3" t="s">
         <v>8</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="2:16">
@@ -3892,16 +4332,16 @@
         <v>1000000</v>
       </c>
       <c r="M55" s="3">
-        <v>229058</v>
+        <v>244951</v>
       </c>
       <c r="N55" s="3">
-        <v>39292</v>
+        <v>31227</v>
       </c>
       <c r="O55" s="3" t="s">
         <v>8</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="2:16">
@@ -3915,53 +4355,151 @@
         <v>1000000</v>
       </c>
       <c r="M56" s="3">
-        <v>716028</v>
+        <v>339636</v>
       </c>
       <c r="N56" s="3">
-        <v>104924</v>
+        <v>40763</v>
       </c>
       <c r="O56" s="3" t="s">
         <v>8</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="2:16">
       <c r="B57" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E57" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16">
+      <c r="M60">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16">
+      <c r="N61" t="s">
+        <v>46</v>
+      </c>
+      <c r="O61">
+        <v>244951</v>
+      </c>
+      <c r="P61">
+        <v>31227</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16">
+      <c r="N62" t="s">
+        <v>43</v>
+      </c>
+      <c r="O62">
+        <v>187385</v>
+      </c>
+      <c r="P62">
+        <v>22721</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16">
+      <c r="N63" t="s">
+        <v>44</v>
+      </c>
+      <c r="O63">
+        <v>161117</v>
+      </c>
+      <c r="P63">
+        <v>19519</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16">
+      <c r="N64" t="s">
+        <v>45</v>
+      </c>
+      <c r="O64">
+        <v>149414</v>
+      </c>
+      <c r="P64">
+        <v>16800</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
+      <c r="N70">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
+      <c r="M72" t="s">
+        <v>43</v>
+      </c>
+      <c r="N72">
+        <v>177638</v>
+      </c>
+      <c r="O72">
+        <v>27768</v>
+      </c>
+      <c r="P72" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
+      <c r="M73" t="s">
+        <v>44</v>
+      </c>
+      <c r="N73">
+        <v>168070</v>
+      </c>
+      <c r="O73">
+        <v>24353</v>
+      </c>
+      <c r="P73" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
+      <c r="J74" s="3"/>
+      <c r="M74" t="s">
+        <v>45</v>
+      </c>
+      <c r="N74">
+        <v>157985</v>
+      </c>
+      <c r="O74">
+        <v>19041</v>
+      </c>
+      <c r="P74" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
       <c r="A76" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B76" s="6"/>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:16">
       <c r="A77" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="I77" s="2"/>
+    </row>
+    <row r="78" spans="1:16">
       <c r="A78" s="8" t="s">
         <v>4</v>
       </c>
@@ -3981,8 +4519,20 @@
         <f>SUM(B78:E78)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="I78" t="s">
+        <v>42</v>
+      </c>
+      <c r="J78">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K78">
+        <v>192916</v>
+      </c>
+      <c r="L78">
+        <v>33295</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16">
       <c r="A79" s="8" t="s">
         <v>9</v>
       </c>
@@ -3990,20 +4540,32 @@
         <v>2</v>
       </c>
       <c r="C79" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D79" s="3">
         <v>2</v>
       </c>
       <c r="E79" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F79" s="9">
         <f t="shared" ref="F79:F81" si="0">SUM(B79:E79)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
+        <v>12</v>
+      </c>
+      <c r="I79" t="s">
+        <v>39</v>
+      </c>
+      <c r="J79">
+        <v>1E-4</v>
+      </c>
+      <c r="K79">
+        <v>192238</v>
+      </c>
+      <c r="L79">
+        <v>33176</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16">
       <c r="A80" s="8" t="s">
         <v>11</v>
       </c>
@@ -4011,72 +4573,114 @@
         <v>4</v>
       </c>
       <c r="C80" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D80" s="3">
         <v>4</v>
       </c>
       <c r="E80" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F80" s="9">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+        <v>12</v>
+      </c>
+      <c r="I80" t="s">
+        <v>40</v>
+      </c>
+      <c r="J80">
+        <v>1E-3</v>
+      </c>
+      <c r="K80">
+        <v>197848</v>
+      </c>
+      <c r="L80">
+        <v>31375</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B81" s="3">
         <v>3</v>
       </c>
       <c r="C81" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D81" s="3">
         <v>3</v>
       </c>
       <c r="E81" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F81" s="9">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+        <v>12</v>
+      </c>
+      <c r="I81" t="s">
+        <v>41</v>
+      </c>
+      <c r="J81">
+        <v>0.01</v>
+      </c>
+      <c r="K81">
+        <v>244951</v>
+      </c>
+      <c r="L81">
+        <v>31227</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="J82">
+        <v>0.1</v>
+      </c>
+      <c r="K82">
+        <v>339636</v>
+      </c>
+      <c r="L82">
+        <v>40763</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="B83" t="s">
+        <v>25</v>
+      </c>
+      <c r="D83" t="s">
+        <v>35</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="K83">
+        <v>411831</v>
+      </c>
+      <c r="L83">
+        <v>48273</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="B84" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="B86" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="B87" t="s">
         <v>29</v>
       </c>
-      <c r="D83" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="B84" t="s">
+    </row>
+    <row r="89" spans="1:12">
+      <c r="B89" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="B86" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="B87" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="B89" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working through first couple function calls for part 1. taking a break
</commit_message>
<xml_diff>
--- a/project03/SimulationOutputs.xlsx
+++ b/project03/SimulationOutputs.xlsx
@@ -2842,16 +2842,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1504950</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3197,8 +3197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I28" workbookViewId="0">
-      <selection activeCell="M56" sqref="M52:M56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>